<commit_message>
Added homework 27 and 28 Feb
</commit_message>
<xml_diff>
--- a/data/0001.xlsx
+++ b/data/0001.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I1229"/>
+  <dimension ref="A1:I1231"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -43489,6 +43489,76 @@
         <v>131700</v>
       </c>
     </row>
+    <row r="1230">
+      <c r="A1230" t="n">
+        <v>1582761600</v>
+      </c>
+      <c r="B1230" t="inlineStr">
+        <is>
+          <t>2020-02-27</t>
+        </is>
+      </c>
+      <c r="C1230" t="inlineStr">
+        <is>
+          <t>0001</t>
+        </is>
+      </c>
+      <c r="D1230" t="inlineStr">
+        <is>
+          <t>SCOMNET</t>
+        </is>
+      </c>
+      <c r="E1230" t="n">
+        <v>0.74</v>
+      </c>
+      <c r="F1230" t="n">
+        <v>0.745</v>
+      </c>
+      <c r="G1230" t="n">
+        <v>0.725</v>
+      </c>
+      <c r="H1230" t="n">
+        <v>0.74</v>
+      </c>
+      <c r="I1230" t="n">
+        <v>429800</v>
+      </c>
+    </row>
+    <row r="1231">
+      <c r="A1231" t="n">
+        <v>1582848000</v>
+      </c>
+      <c r="B1231" t="inlineStr">
+        <is>
+          <t>2020-02-28</t>
+        </is>
+      </c>
+      <c r="C1231" t="inlineStr">
+        <is>
+          <t>0001</t>
+        </is>
+      </c>
+      <c r="D1231" t="inlineStr">
+        <is>
+          <t>SCOMNET</t>
+        </is>
+      </c>
+      <c r="E1231" t="n">
+        <v>0.725</v>
+      </c>
+      <c r="F1231" t="n">
+        <v>0.73</v>
+      </c>
+      <c r="G1231" t="n">
+        <v>0.6899999999999999</v>
+      </c>
+      <c r="H1231" t="n">
+        <v>0.705</v>
+      </c>
+      <c r="I1231" t="n">
+        <v>1047600</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added homework 12 March 20
</commit_message>
<xml_diff>
--- a/data/0001.xlsx
+++ b/data/0001.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I1239"/>
+  <dimension ref="A1:I1240"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -43839,6 +43839,41 @@
         <v>167500</v>
       </c>
     </row>
+    <row r="1240">
+      <c r="A1240" t="n">
+        <v>1583971200</v>
+      </c>
+      <c r="B1240" t="inlineStr">
+        <is>
+          <t>2020-03-12</t>
+        </is>
+      </c>
+      <c r="C1240" t="inlineStr">
+        <is>
+          <t>0001</t>
+        </is>
+      </c>
+      <c r="D1240" t="inlineStr">
+        <is>
+          <t>SCOMNET</t>
+        </is>
+      </c>
+      <c r="E1240" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="F1240" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="G1240" t="n">
+        <v>0.57</v>
+      </c>
+      <c r="H1240" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="I1240" t="n">
+        <v>464300</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>